<commit_message>
Fixed columnn name issue for infantlanglab_utk, and re-ran 01_ script
</commit_message>
<xml_diff>
--- a/processed_data/handcoded_cleaned/infantlanglab_utk_trials_gazefollowing.xlsx
+++ b/processed_data/handcoded_cleaned/infantlanglab_utk_trials_gazefollowing.xlsx
@@ -1,15 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krista/Repos/gaze-following-analysis/processed_data/handcoded_cleaned/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AE83F3-3CA7-E947-A51E-543080F46FCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12160"/>
+    <workbookView xWindow="5920" yWindow="560" windowWidth="25600" windowHeight="12160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="infantlanglab_utk_trials_gazefo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">infantlanglab_utk_trials_gazefo!$A$1:$M$211</definedName>
+  </definedNames>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -261,7 +270,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1088,21 +1097,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
@@ -1117,7 +1126,7 @@
     <col min="13" max="13" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1158,7 +1167,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1363,7 +1372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1486,7 +1495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1527,7 +1536,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1609,7 +1618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1650,7 +1659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1691,7 +1700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1773,7 +1782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1814,7 +1823,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1855,7 +1864,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1896,7 +1905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1937,7 +1946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1978,7 +1987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -2060,7 +2069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -2101,7 +2110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2142,7 +2151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2183,7 +2192,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -2265,7 +2274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2347,7 +2356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2388,7 +2397,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2470,7 +2479,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2511,7 +2520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2593,7 +2602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2634,7 +2643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2675,7 +2684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2716,7 +2725,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -2757,7 +2766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2798,7 +2807,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2839,7 +2848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2880,7 +2889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2921,7 +2930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2962,7 +2971,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3044,7 +3053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
@@ -3085,7 +3094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -3126,7 +3135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -3208,7 +3217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>11</v>
       </c>
@@ -3249,7 +3258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -3290,7 +3299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -3331,7 +3340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -3372,7 +3381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>11</v>
       </c>
@@ -3413,7 +3422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>11</v>
       </c>
@@ -3454,7 +3463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>11</v>
       </c>
@@ -3495,7 +3504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -3536,7 +3545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>11</v>
       </c>
@@ -3577,7 +3586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>11</v>
       </c>
@@ -3618,7 +3627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -3659,7 +3668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -3700,7 +3709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -3741,7 +3750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -3782,7 +3791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -3823,7 +3832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -3864,7 +3873,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -3905,7 +3914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -3946,7 +3955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -3987,7 +3996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -4028,7 +4037,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -4069,7 +4078,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -4110,7 +4119,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -4151,7 +4160,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -4192,7 +4201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -4233,7 +4242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -4315,7 +4324,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -4356,7 +4365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -4397,7 +4406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -4438,7 +4447,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -4479,7 +4488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -4520,7 +4529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -4561,7 +4570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -4602,7 +4611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -4643,7 +4652,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -4684,7 +4693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -4725,7 +4734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -4766,7 +4775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -4807,7 +4816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -4848,7 +4857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -4889,7 +4898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -4930,7 +4939,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -4971,7 +4980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -5012,7 +5021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -5053,7 +5062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -5094,7 +5103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -5135,7 +5144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -5176,7 +5185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -5217,7 +5226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -5258,7 +5267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -5299,7 +5308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -5340,7 +5349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -5381,7 +5390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -5422,7 +5431,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -5463,7 +5472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -5504,7 +5513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -5545,7 +5554,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -5586,7 +5595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -5627,7 +5636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -5668,7 +5677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -5709,7 +5718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -5750,7 +5759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -5791,7 +5800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -5832,7 +5841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -5873,7 +5882,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -5914,7 +5923,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -5955,7 +5964,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -5996,7 +6005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -6037,7 +6046,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -6078,7 +6087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -6119,7 +6128,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -6160,7 +6169,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -6201,7 +6210,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -6242,7 +6251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -6283,7 +6292,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -6324,7 +6333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -6365,7 +6374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -6406,7 +6415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -6447,7 +6456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -6488,7 +6497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -6529,7 +6538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -6570,7 +6579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -6611,7 +6620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -6652,7 +6661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -6693,7 +6702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -6734,7 +6743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -6775,7 +6784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>11</v>
       </c>
@@ -6816,7 +6825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -6857,7 +6866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -6898,7 +6907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -6939,7 +6948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -6980,7 +6989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -7021,7 +7030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -7062,7 +7071,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -7103,7 +7112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -7144,7 +7153,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -7185,7 +7194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -7226,7 +7235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -7267,7 +7276,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -7308,7 +7317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -7349,7 +7358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -7390,7 +7399,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -7431,7 +7440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -7472,7 +7481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -7513,7 +7522,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>11</v>
       </c>
@@ -7554,7 +7563,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -7595,7 +7604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>11</v>
       </c>
@@ -7636,7 +7645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -7677,7 +7686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>11</v>
       </c>
@@ -7718,7 +7727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -7759,7 +7768,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>11</v>
       </c>
@@ -7800,7 +7809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>11</v>
       </c>
@@ -7841,7 +7850,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>11</v>
       </c>
@@ -7882,7 +7891,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>11</v>
       </c>
@@ -7923,7 +7932,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>11</v>
       </c>
@@ -7964,7 +7973,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -8005,7 +8014,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>11</v>
       </c>
@@ -8046,7 +8055,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>11</v>
       </c>
@@ -8087,7 +8096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>11</v>
       </c>
@@ -8128,7 +8137,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>11</v>
       </c>
@@ -8169,7 +8178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>11</v>
       </c>
@@ -8210,7 +8219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -8251,7 +8260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -8292,7 +8301,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -8333,7 +8342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>11</v>
       </c>
@@ -8374,7 +8383,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>11</v>
       </c>
@@ -8415,7 +8424,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>11</v>
       </c>
@@ -8456,7 +8465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>11</v>
       </c>
@@ -8497,7 +8506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>11</v>
       </c>
@@ -8538,7 +8547,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>11</v>
       </c>
@@ -8579,7 +8588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>11</v>
       </c>
@@ -8620,7 +8629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>11</v>
       </c>
@@ -8661,7 +8670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -8702,7 +8711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -8743,7 +8752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -8784,7 +8793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>11</v>
       </c>
@@ -8825,7 +8834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -8866,7 +8875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -8907,7 +8916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -8948,7 +8957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -8989,7 +8998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -9030,7 +9039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>11</v>
       </c>
@@ -9071,7 +9080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>11</v>
       </c>
@@ -9112,7 +9121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>11</v>
       </c>
@@ -9153,7 +9162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>11</v>
       </c>
@@ -9194,7 +9203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>11</v>
       </c>
@@ -9235,7 +9244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>11</v>
       </c>
@@ -9276,7 +9285,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>11</v>
       </c>
@@ -9317,7 +9326,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>11</v>
       </c>
@@ -9358,7 +9367,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>11</v>
       </c>
@@ -9399,7 +9408,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -9440,7 +9449,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>11</v>
       </c>
@@ -9481,7 +9490,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>11</v>
       </c>
@@ -9522,7 +9531,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -9563,7 +9572,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>11</v>
       </c>
@@ -9604,7 +9613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>11</v>
       </c>
@@ -9645,7 +9654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>11</v>
       </c>
@@ -9686,7 +9695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>11</v>
       </c>
@@ -9727,7 +9736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -9769,6 +9778,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M211" xr:uid="{D51021C1-C3BC-6E48-9A26-208CA2EA7B1F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>